<commit_message>
Deploying to gh-pages from @ matthewdlang18/macroeconomics-course-website@463cf30efb0570c4a3cf63f91a7050638654af6d 🚀
</commit_message>
<xml_diff>
--- a/course_materials/GDP.xlsx
+++ b/course_materials/GDP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattlang/Cursor/macroeconomics-course-website/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0B5C1A-6A12-7D42-A7AE-6DA6B5CC541C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1116A207-E4A5-2E4F-BC55-5C96D176E3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="1540" windowWidth="29120" windowHeight="18880" xr2:uid="{32AFCFF0-4E69-B847-A58D-E17547420AE6}"/>
+    <workbookView xWindow="32260" yWindow="1520" windowWidth="27740" windowHeight="18880" activeTab="1" xr2:uid="{32AFCFF0-4E69-B847-A58D-E17547420AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Nominal GDP" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5459" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5460" uniqueCount="340">
   <si>
     <t>1947Q1</t>
   </si>
@@ -1055,6 +1055,9 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
 </sst>
 </file>
 
@@ -1430,7 +1433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3E0E7F-AFBF-8043-8218-597DCDC29649}">
   <dimension ref="A1:G313"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A304" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -8642,10 +8645,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FF1A7A-728D-274C-90DB-35E537798C7A}">
-  <dimension ref="A1:AB313"/>
+  <dimension ref="A1:AB314"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC314" sqref="AC314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35568,6 +35572,92 @@
         <v>-34970</v>
       </c>
     </row>
+    <row r="314" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>339</v>
+      </c>
+      <c r="B314" s="1">
+        <v>23526100</v>
+      </c>
+      <c r="C314" s="1">
+        <v>16345600</v>
+      </c>
+      <c r="D314" s="1">
+        <v>5567400</v>
+      </c>
+      <c r="E314" s="1">
+        <v>2102400</v>
+      </c>
+      <c r="F314" s="1">
+        <v>3476200</v>
+      </c>
+      <c r="G314" s="1">
+        <v>10800000</v>
+      </c>
+      <c r="H314" s="1">
+        <v>4533700</v>
+      </c>
+      <c r="I314" s="1">
+        <v>4346800</v>
+      </c>
+      <c r="J314" s="1">
+        <v>3595500</v>
+      </c>
+      <c r="K314" s="1">
+        <v>677000</v>
+      </c>
+      <c r="L314" s="1">
+        <v>1399600</v>
+      </c>
+      <c r="M314" s="1">
+        <v>1522500</v>
+      </c>
+      <c r="N314" s="1">
+        <v>799600</v>
+      </c>
+      <c r="O314" s="1">
+        <v>140100</v>
+      </c>
+      <c r="P314" s="1">
+        <v>-1374300</v>
+      </c>
+      <c r="Q314" s="1">
+        <v>2648800</v>
+      </c>
+      <c r="R314" s="1">
+        <v>1752000</v>
+      </c>
+      <c r="S314" s="1">
+        <v>899600</v>
+      </c>
+      <c r="T314" s="1">
+        <v>4023100</v>
+      </c>
+      <c r="U314" s="1">
+        <v>3311500</v>
+      </c>
+      <c r="V314" s="1">
+        <v>714500</v>
+      </c>
+      <c r="W314" s="1">
+        <v>3981700</v>
+      </c>
+      <c r="X314" s="1">
+        <v>1515100</v>
+      </c>
+      <c r="Y314" s="1">
+        <v>858000</v>
+      </c>
+      <c r="Z314" s="1">
+        <v>657000</v>
+      </c>
+      <c r="AA314" s="1">
+        <v>2465300</v>
+      </c>
+      <c r="AB314" s="1">
+        <v>-117600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ matthewdlang18/macroeconomics-course-website@b2b6d3ecd6a2c5ce6e976fa66bb431c3689ec309 🚀
</commit_message>
<xml_diff>
--- a/course_materials/GDP.xlsx
+++ b/course_materials/GDP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattlang/Cursor/macroeconomics-course-website/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1116A207-E4A5-2E4F-BC55-5C96D176E3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F63F37-38B0-304A-980A-D5AC39EEE2BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32260" yWindow="1520" windowWidth="27740" windowHeight="18880" activeTab="1" xr2:uid="{32AFCFF0-4E69-B847-A58D-E17547420AE6}"/>
+    <workbookView xWindow="10800" yWindow="760" windowWidth="18420" windowHeight="18880" xr2:uid="{32AFCFF0-4E69-B847-A58D-E17547420AE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Nominal GDP" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5460" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5461" uniqueCount="340">
   <si>
     <t>1947Q1</t>
   </si>
@@ -1063,10 +1063,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1431,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3E0E7F-AFBF-8043-8218-597DCDC29649}">
-  <dimension ref="A1:G313"/>
+  <dimension ref="A1:G314"/>
   <sheetViews>
-    <sheetView topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="A314" sqref="A314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8638,7 +8644,31 @@
         <v>5099730</v>
       </c>
     </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>339</v>
+      </c>
+      <c r="B314" s="1">
+        <v>29977500</v>
+      </c>
+      <c r="C314" s="1">
+        <v>20526300</v>
+      </c>
+      <c r="D314" s="1">
+        <v>5573200</v>
+      </c>
+      <c r="E314" s="1">
+        <v>3276400</v>
+      </c>
+      <c r="F314" s="1">
+        <v>-4538700</v>
+      </c>
+      <c r="G314" s="1">
+        <v>3941800</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8647,7 +8677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FF1A7A-728D-274C-90DB-35E537798C7A}">
   <dimension ref="A1:AB314"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AC314" sqref="AC314"/>
     </sheetView>

</xml_diff>